<commit_message>
Created better looking graphs and deleted many unnecessary ones
</commit_message>
<xml_diff>
--- a/data/NACE.xlsx
+++ b/data/NACE.xlsx
@@ -32,9 +32,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>Agriculture, Forestry, and Fishing</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -62,30 +59,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>Mining and Quarrying</t>
-  </si>
-  <si>
-    <t>Manufacturing</t>
-  </si>
-  <si>
-    <t>Electricity, Gas, Steam, and Air Conditioning Supply</t>
-  </si>
-  <si>
-    <t>Water Supply, Sewerage, Waste Management, and Remediation Activities</t>
-  </si>
-  <si>
-    <t>Construction</t>
-  </si>
-  <si>
-    <t>Wholesale and Retail Trade; Repair of Motor Vehicles and Motorcycles</t>
-  </si>
-  <si>
-    <t>Transportation and Storage</t>
-  </si>
-  <si>
-    <t>Accommodation and Food Service Activities</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -122,46 +95,73 @@
     <t>U</t>
   </si>
   <si>
-    <t>Information and Communication</t>
-  </si>
-  <si>
-    <t>Financial and Insurance Activities</t>
-  </si>
-  <si>
-    <t>Real Estate Activities</t>
-  </si>
-  <si>
-    <t>Professional, Scientific, and Technical Activities</t>
-  </si>
-  <si>
-    <t>Administrative and Support Service Activities</t>
-  </si>
-  <si>
-    <t>Public Administration and Defence; Compulsory Social Security</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>Human Health and Social Work Activities</t>
-  </si>
-  <si>
-    <t>Arts, Entertainment, and Recreation</t>
-  </si>
-  <si>
-    <t>Other Service Activities</t>
-  </si>
-  <si>
-    <t>Activities of Households as Employers; Undifferentiated Goods- and Services-Producing Activities of Households for Own Use</t>
-  </si>
-  <si>
-    <t>Activities of Extraterritorial Organizations and Bodies</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>Other</t>
+    <t>A. Agriculture, Forestry, and Fishing</t>
+  </si>
+  <si>
+    <t>B. Mining and Quarrying</t>
+  </si>
+  <si>
+    <t>C. Manufacturing</t>
+  </si>
+  <si>
+    <t>D. Electricity, Gas, Steam, and Air Conditioning Supply</t>
+  </si>
+  <si>
+    <t>E. Water Supply, Sewerage, Waste Management, and Remediation Activities</t>
+  </si>
+  <si>
+    <t>F. Construction</t>
+  </si>
+  <si>
+    <t>G. Wholesale and Retail Trade; Repair of Motor Vehicles and Motorcycles</t>
+  </si>
+  <si>
+    <t>H. Transportation and Storage</t>
+  </si>
+  <si>
+    <t>I. Accommodation and Food Service Activities</t>
+  </si>
+  <si>
+    <t>J. Information and Communication</t>
+  </si>
+  <si>
+    <t>K. Financial and Insurance Activities</t>
+  </si>
+  <si>
+    <t>L. Real Estate Activities</t>
+  </si>
+  <si>
+    <t>M. Professional, Scientific, and Technical Activities</t>
+  </si>
+  <si>
+    <t>N. Administrative and Support Service Activities</t>
+  </si>
+  <si>
+    <t>O. Public Administration and Defence; Compulsory Social Security</t>
+  </si>
+  <si>
+    <t>P. Education</t>
+  </si>
+  <si>
+    <t>Q. Human Health and Social Work Activities</t>
+  </si>
+  <si>
+    <t>R. Arts, Entertainment, and Recreation</t>
+  </si>
+  <si>
+    <t>S. Other Service Activities</t>
+  </si>
+  <si>
+    <t>T. Activities of Households as Employers; Undifferentiated Goods- and Services-Producing Activities of Households for Own Use</t>
+  </si>
+  <si>
+    <t>U. Activities of Extraterritorial Organizations and Bodies</t>
+  </si>
+  <si>
+    <t>X. Other</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -497,175 +497,175 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
some new data and images added
</commit_message>
<xml_diff>
--- a/data/NACE.xlsx
+++ b/data/NACE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sortizgu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A272BB-AEB3-4533-B048-1A5FF6A8B15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -107,18 +108,9 @@
     <t>C. Manufacturing</t>
   </si>
   <si>
-    <t>D. Electricity, Gas, Steam, and Air Conditioning Supply</t>
-  </si>
-  <si>
-    <t>E. Water Supply, Sewerage, Waste Management, and Remediation Activities</t>
-  </si>
-  <si>
     <t>F. Construction</t>
   </si>
   <si>
-    <t>G. Wholesale and Retail Trade; Repair of Motor Vehicles and Motorcycles</t>
-  </si>
-  <si>
     <t>H. Transportation and Storage</t>
   </si>
   <si>
@@ -134,9 +126,6 @@
     <t>L. Real Estate Activities</t>
   </si>
   <si>
-    <t>M. Professional, Scientific, and Technical Activities</t>
-  </si>
-  <si>
     <t>N. Administrative and Support Service Activities</t>
   </si>
   <si>
@@ -146,9 +135,6 @@
     <t>P. Education</t>
   </si>
   <si>
-    <t>Q. Human Health and Social Work Activities</t>
-  </si>
-  <si>
     <t>R. Arts, Entertainment, and Recreation</t>
   </si>
   <si>
@@ -162,12 +148,27 @@
   </si>
   <si>
     <t>X. Other</t>
+  </si>
+  <si>
+    <t>G. Wholesale and Retail Trade</t>
+  </si>
+  <si>
+    <t>D. Energy Supply</t>
+  </si>
+  <si>
+    <t>E. Water Supply, and Remediation Activities</t>
+  </si>
+  <si>
+    <t>M. Professional Activities</t>
+  </si>
+  <si>
+    <t>Q. Health Care</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,14 +479,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -524,7 +525,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -532,7 +533,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -540,7 +541,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -548,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -556,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -564,7 +565,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -572,7 +573,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -580,7 +581,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -588,7 +589,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -596,7 +597,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -604,7 +605,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -612,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -620,7 +621,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -628,7 +629,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -636,7 +637,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -644,7 +645,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -652,7 +653,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -660,7 +661,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -668,7 +669,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>